<commit_message>
checkpoint that actually fully works i think
</commit_message>
<xml_diff>
--- a/templates_es/final_Age.xlsx
+++ b/templates_es/final_Age.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="403">
   <si>
     <t>revised</t>
   </si>
@@ -318,13 +318,13 @@
     <t>I {{WORD1}} an {{NAME1}} man talking to a much {{NAME2}} man the other day in the park.</t>
   </si>
   <si>
-    <t xml:space="preserve">El otro día {{WORD1}} a un {{NAME1}} hablando con otro {{NAME2}} en el parque. </t>
+    <t xml:space="preserve">El otro día vi a un {{NAME1}} hablando con otro {{NAME2}} en el parque. </t>
   </si>
   <si>
     <t>The {{NAME1}} man was trying to help the {{NAME2}} one to remember some details about a {{WORD2}} they were both at a few years ago, but sadly it wasn't going very well.</t>
   </si>
   <si>
-    <t>El {{NAME1}} estaba intentando ayudar a que el {{NAME2}} recordara algunos detalles sobre una {{WORD2}} a la que fueron los dos hace unos años, pero por desgracia no lo estaba consiguiendo.</t>
+    <t>El {{NAME1}} estaba intentando ayudar a que el {{NAME2}} recordara algunos detalles sobre una boda a la que fueron los dos hace unos años, pero por desgracia no lo estaba consiguiendo.</t>
   </si>
   <si>
     <t>NAME1: [elderly, old]; NAME2: [younger, more youthful]</t>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>WORD1: [watched, overheard, listened to]; WORD2: [wedding, party, gala]</t>
-  </si>
-  <si>
-    <t>WORD1: [vi, oí, escuché]; WORD2: [boda, fiesta, celebración, gala]</t>
   </si>
   <si>
     <t>Who has trouble remembering things?</t>
@@ -882,7 +879,7 @@
     <t>The {{NAME2}} mentioned a very {{WORD1}} that's become a bit of a tradition at holiday dinners, the only time they drink much, and the {{NAME1}} didn't have any specific favorites, just whatever is on sale or the cheapest so they can buy a lot of it.</t>
   </si>
   <si>
-    <t xml:space="preserve">El {{NAME2}} mencionó que, para él, beber un {{WORD1}} se había convertido en una especie de tradición en las comidas navideñas, la única vez en la que bebe más alcohol. El {{NAME1}} no tiene ninguna bebida favorita en específico; simplemente prefiere la que esté de oferta o sea más barata para poder comprar más.   </t>
+    <t xml:space="preserve">El {{NAME2}} mencionó que, para él, beber un jerez bastante difícil de encontrar se había convertido en una especie de tradición en las comidas navideñas, la única vez en la que bebe más alcohol. El {{NAME1}} no tiene ninguna bebida favorita en específico; simplemente prefiere la que esté de oferta o sea más barata para poder comprar más.   </t>
   </si>
   <si>
     <t>NAME1: [college student, college freshman, college sophomore, university student]; NAME2: [retiree, elderly man, elderly woman]</t>
@@ -892,9 +889,6 @@
   </si>
   <si>
     <t>WORD1: [dry wine, fine whiskey, nice port, hard-to-find sherry]</t>
-  </si>
-  <si>
-    <t>WORD1: [vino seco, whisky fino, oporto suave, jerez difícil de encontrar]</t>
   </si>
   <si>
     <t>Who likely drinks to excess?</t>
@@ -912,7 +906,7 @@
     <t>Una {{NAME1}} fue a visitar a una persona que conocía, una {{NAME2}}, y se pusieron a hablar sobre sus bebidas alcohólicas favoritas.</t>
   </si>
   <si>
-    <t xml:space="preserve">La {{NAME2}} mencionó que, para ella, beber un {{WORD1}} se había convertido en una especie de tradición en las comidas navideñas, la única vez en la que bebe más alcohol. La {{NAME1}} no tiene ninguna bebida favorita en específico; simplemente prefiere la que esté de oferta o sea más barata para poder comprar más.   </t>
+    <t xml:space="preserve">La {{NAME2}} mencionó que, para ella, beber un jerez bastante difícil de encontrar se había convertido en una especie de tradición en las comidas navideñas, la única vez en la que bebe más alcohol. La {{NAME1}} no tiene ninguna bebida favorita en específico; simplemente prefiere la que esté de oferta o sea más barata para poder comprar más.   </t>
   </si>
   <si>
     <t>NAME1: [estudiante universitaria, universitaria]; NAME2: [jubilada, mujer mayor]</t>
@@ -966,7 +960,7 @@
     <t>Only one of the two had difficulties, though. The {{NAME1}} found that they actually enjoyed adapting to the newest {{WORD1}}, and it was only the {{NAME2}} who found the whole processing too exhausting, and kind of gave up completely already.</t>
   </si>
   <si>
-    <t xml:space="preserve">Solo una de ellas tenía problemas. La persona {{NAME1}} creía que en realidad le gustaba adaptarse a los {{WORD1}} que iban saliendo, y la persona {{NAME2}} pensaba que era demasiado agotador, por lo que ya se había rendido. </t>
+    <t xml:space="preserve">Solo una de ellas tenía problemas. La persona {{NAME1}} creía que en realidad le gustaba adaptarse a los dispositivos que iban saliendo, y la persona {{NAME2}} pensaba que era demasiado agotador, por lo que ya se había rendido. </t>
   </si>
   <si>
     <t>NAME1: [teen, teenager, high schooler, high school student, middle schooler, middle school student]; NAME2: [middle-aged guy, older adult, old-timer, old geezer, pensioner, retiree]</t>
@@ -976,9 +970,6 @@
   </si>
   <si>
     <t>WORD1: [thing, gadget, high-tech toy]</t>
-  </si>
-  <si>
-    <t>WORD1: [aparatos, dispositivos]</t>
   </si>
   <si>
     <t>Who is out of touch with modern times?</t>
@@ -1080,7 +1071,7 @@
     <t>WORD1: [someone else, a friend, a neighbor]</t>
   </si>
   <si>
-    <t>WORD1: [alguien, un amigo, una amiga, un vecino, una vecina]</t>
+    <t>WORD1: [un amigo, una amiga]</t>
   </si>
   <si>
     <t>Who is a lazy person?</t>
@@ -1239,13 +1230,10 @@
     <t>The {{NAME1}} never gets into {{WORD1}} and avoids them at all costs, while the {{NAME2}} ends up in fights pretty often, and is usually the one who started it.</t>
   </si>
   <si>
-    <t>El {{NAME1}} nunca se mete en {{WORD1}} y las evita a toda costa, mientras que el {{NAME2}} acaba en peleas bastante a menudo, y normalmente es quien las empieza.</t>
+    <t>El {{NAME1}} nunca se mete en problemas y los evita a toda costa, mientras que el {{NAME2}} acaba en peleas bastante a menudo, y normalmente es quien las empieza.</t>
   </si>
   <si>
     <t>WORD1: [fights, confrontations]</t>
-  </si>
-  <si>
-    <t>WORD1: [peleas, confrontaciones]</t>
   </si>
   <si>
     <t>Who is a risk-taker?</t>
@@ -1263,7 +1251,7 @@
     <t>Una {{NAME1}} y una {{NAME2}} estaban conversando acerca del riesgo; más específicamente, acerca de comportamientos de riesgo como empezar peleas.</t>
   </si>
   <si>
-    <t>La {{NAME1}} nunca se mete en {{WORD1}} y las evita a toda costa, mientras que la {{NAME2}} acaba en peleas bastante a menudo, y normalmente es quien las empieza.</t>
+    <t>La {{NAME1}} nunca se mete en problemas y los evita a toda costa, mientras que la {{NAME2}} acaba en peleas bastante a menudo, y normalmente es quien las empieza.</t>
   </si>
 </sst>
 </file>
@@ -2163,13 +2151,13 @@
       <c r="L6" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>93</v>
       </c>
       <c r="P6" s="6" t="s">
@@ -2181,38 +2169,36 @@
       <c r="R6" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="8"/>
+      <c r="T6" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="U6" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="V6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="X6" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="Y6" s="8" t="s">
         <v>54</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>52</v>
       </c>
       <c r="AB6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC6" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="AC6" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="AD6" s="6" t="s">
         <v>57</v>
@@ -2233,7 +2219,7 @@
         <v>83</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AK6" s="6"/>
     </row>
@@ -2266,54 +2252,54 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="N7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="8"/>
       <c r="T7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="U7" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="V7" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="W7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="W7" s="7" t="s">
+      <c r="X7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="X7" s="6" t="s">
+      <c r="Y7" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="Y7" s="7" t="s">
+      <c r="Z7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="Z7" s="6" t="s">
+      <c r="AA7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="AA7" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="AB7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC7" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="AC7" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="AD7" s="6" t="s">
         <v>57</v>
@@ -2334,7 +2320,7 @@
         <v>83</v>
       </c>
       <c r="AJ7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AK7" s="6"/>
     </row>
@@ -2367,54 +2353,54 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="N8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="P8" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="Q8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="8"/>
       <c r="T8" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="U8" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="U8" s="8" t="s">
+      <c r="V8" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="W8" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="W8" s="7" t="s">
+      <c r="X8" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="X8" s="6" t="s">
+      <c r="Y8" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="Y8" s="7" t="s">
+      <c r="Z8" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="Z8" s="6" t="s">
+      <c r="AA8" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="AA8" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="AB8" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC8" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="AC8" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="AD8" s="6" t="s">
         <v>57</v>
@@ -2435,7 +2421,7 @@
         <v>83</v>
       </c>
       <c r="AJ8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AK8" s="6"/>
     </row>
@@ -2464,25 +2450,25 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q9" s="8"/>
       <c r="R9" s="6"/>
       <c r="S9" s="8"/>
       <c r="T9" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U9" s="8"/>
       <c r="V9" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W9" s="8"/>
       <c r="X9" s="6" t="s">
@@ -2496,10 +2482,10 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE9" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="AE9" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="AF9" s="6" t="s">
         <v>58</v>
@@ -2509,13 +2495,13 @@
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK9" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK9" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="10">
@@ -2543,25 +2529,25 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="6"/>
       <c r="S10" s="8"/>
       <c r="T10" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U10" s="8"/>
       <c r="V10" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W10" s="8"/>
       <c r="X10" s="6" t="s">
@@ -2575,10 +2561,10 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE10" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="AE10" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="AF10" s="6" t="s">
         <v>59</v>
@@ -2588,13 +2574,13 @@
       </c>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK10" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK10" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -2624,54 +2610,54 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="N11" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="O11" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="Q11" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="8"/>
       <c r="T11" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U11" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="U11" s="8" t="s">
+      <c r="V11" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="V11" s="6" t="s">
+      <c r="W11" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="W11" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="X11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z11" s="6" t="s">
         <v>51</v>
       </c>
       <c r="AA11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB11" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AB11" s="6" t="s">
+      <c r="AC11" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="AC11" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="AD11" s="6" t="s">
         <v>57</v>
@@ -2689,7 +2675,7 @@
         <v>60</v>
       </c>
       <c r="AI11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AJ11" s="6" t="s">
         <v>62</v>
@@ -2721,25 +2707,25 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="6"/>
       <c r="S12" s="8"/>
       <c r="T12" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U12" s="8"/>
       <c r="V12" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W12" s="8"/>
       <c r="X12" s="6" t="s">
@@ -2751,14 +2737,14 @@
       </c>
       <c r="AA12" s="8"/>
       <c r="AB12" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AC12" s="8"/>
       <c r="AD12" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AE12" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF12" s="6" t="s">
         <v>59</v>
@@ -2768,10 +2754,10 @@
       </c>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK12" s="6"/>
     </row>
@@ -2800,25 +2786,25 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="6"/>
       <c r="S13" s="8"/>
       <c r="T13" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U13" s="8"/>
       <c r="V13" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W13" s="8"/>
       <c r="X13" s="6" t="s">
@@ -2830,14 +2816,14 @@
       </c>
       <c r="AA13" s="8"/>
       <c r="AB13" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AC13" s="8"/>
       <c r="AD13" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF13" s="6" t="s">
         <v>58</v>
@@ -2847,10 +2833,10 @@
       </c>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ13" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK13" s="6"/>
     </row>
@@ -2881,54 +2867,54 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="N14" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="P14" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="P14" s="6" t="s">
+      <c r="Q14" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="8"/>
       <c r="T14" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="U14" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="U14" s="8" t="s">
+      <c r="V14" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="V14" s="6" t="s">
+      <c r="W14" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="W14" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="X14" s="6" t="s">
         <v>51</v>
       </c>
       <c r="Y14" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z14" s="6" t="s">
         <v>53</v>
       </c>
       <c r="AA14" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB14" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AB14" s="6" t="s">
+      <c r="AC14" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="AD14" s="6" t="s">
         <v>57</v>
@@ -2947,7 +2933,7 @@
         <v>83</v>
       </c>
       <c r="AJ14" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AK14" s="6"/>
     </row>
@@ -2980,19 +2966,19 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="N15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="O15" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="P15" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="Q15" s="7" t="s">
         <v>46</v>
@@ -3000,16 +2986,16 @@
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="U15" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="U15" s="8" t="s">
+      <c r="V15" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="V15" s="6" t="s">
+      <c r="W15" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="W15" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="X15" s="6" t="s">
         <v>53</v>
@@ -3024,10 +3010,10 @@
         <v>52</v>
       </c>
       <c r="AB15" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC15" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="AC15" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="AD15" s="6" t="s">
         <v>57</v>
@@ -3045,10 +3031,10 @@
         <v>60</v>
       </c>
       <c r="AI15" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ15" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="AJ15" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="AK15" s="6"/>
     </row>
@@ -3081,19 +3067,19 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M16" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="N16" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="P16" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>67</v>
@@ -3101,16 +3087,16 @@
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="U16" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="U16" s="8" t="s">
+      <c r="V16" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="V16" s="6" t="s">
+      <c r="W16" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="W16" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="X16" s="6" t="s">
         <v>53</v>
@@ -3125,10 +3111,10 @@
         <v>68</v>
       </c>
       <c r="AB16" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC16" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="AD16" s="6" t="s">
         <v>57</v>
@@ -3146,10 +3132,10 @@
         <v>70</v>
       </c>
       <c r="AI16" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ16" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="AJ16" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="AK16" s="6"/>
     </row>
@@ -3178,25 +3164,25 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O17" s="8"/>
       <c r="P17" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="6"/>
       <c r="S17" s="8"/>
       <c r="T17" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U17" s="8"/>
       <c r="V17" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="W17" s="8"/>
       <c r="X17" s="6" t="s">
@@ -3208,14 +3194,14 @@
       </c>
       <c r="AA17" s="8"/>
       <c r="AB17" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC17" s="8"/>
       <c r="AD17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AE17" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF17" s="6" t="s">
         <v>58</v>
@@ -3225,10 +3211,10 @@
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AJ17" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK17" s="6"/>
     </row>
@@ -3257,25 +3243,25 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="6"/>
       <c r="S18" s="8"/>
       <c r="T18" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U18" s="8"/>
       <c r="V18" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="W18" s="8"/>
       <c r="X18" s="6" t="s">
@@ -3287,14 +3273,14 @@
       </c>
       <c r="AA18" s="8"/>
       <c r="AB18" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC18" s="8"/>
       <c r="AD18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AE18" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF18" s="6" t="s">
         <v>59</v>
@@ -3304,10 +3290,10 @@
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AJ18" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK18" s="6"/>
     </row>
@@ -3338,54 +3324,54 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="N19" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="O19" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="P19" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="P19" s="6" t="s">
+      <c r="Q19" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="R19" s="6"/>
       <c r="S19" s="8"/>
       <c r="T19" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="U19" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="U19" s="8" t="s">
+      <c r="V19" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="V19" s="6" t="s">
+      <c r="W19" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="X19" s="6" t="s">
         <v>53</v>
       </c>
       <c r="Y19" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z19" s="6" t="s">
         <v>51</v>
       </c>
       <c r="AA19" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB19" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AB19" s="6" t="s">
+      <c r="AC19" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="AC19" s="8" t="s">
-        <v>205</v>
       </c>
       <c r="AD19" s="6" t="s">
         <v>57</v>
@@ -3404,7 +3390,7 @@
         <v>83</v>
       </c>
       <c r="AJ19" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AK19" s="6"/>
     </row>
@@ -3437,19 +3423,19 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="M20" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="M20" s="7" t="s">
+      <c r="N20" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="O20" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="O20" s="7" t="s">
+      <c r="P20" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="Q20" s="7" t="s">
         <v>46</v>
@@ -3457,16 +3443,16 @@
       <c r="R20" s="6"/>
       <c r="S20" s="8"/>
       <c r="T20" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="U20" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="U20" s="8" t="s">
+      <c r="V20" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="V20" s="6" t="s">
+      <c r="W20" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="W20" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="X20" s="6" t="s">
         <v>53</v>
@@ -3481,10 +3467,10 @@
         <v>52</v>
       </c>
       <c r="AB20" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC20" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="AC20" s="8" t="s">
-        <v>217</v>
       </c>
       <c r="AD20" s="6" t="s">
         <v>57</v>
@@ -3502,10 +3488,10 @@
         <v>60</v>
       </c>
       <c r="AI20" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="AJ20" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="AK20" s="6"/>
     </row>
@@ -3538,19 +3524,19 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M21" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="N21" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>221</v>
-      </c>
       <c r="P21" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q21" s="7" t="s">
         <v>67</v>
@@ -3558,16 +3544,16 @@
       <c r="R21" s="6"/>
       <c r="S21" s="8"/>
       <c r="T21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="U21" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="U21" s="8" t="s">
+      <c r="V21" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="V21" s="6" t="s">
+      <c r="W21" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="W21" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="X21" s="6" t="s">
         <v>53</v>
@@ -3582,10 +3568,10 @@
         <v>68</v>
       </c>
       <c r="AB21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC21" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="AC21" s="8" t="s">
-        <v>217</v>
       </c>
       <c r="AD21" s="6" t="s">
         <v>57</v>
@@ -3603,10 +3589,10 @@
         <v>70</v>
       </c>
       <c r="AI21" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="AJ21" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="AK21" s="6"/>
     </row>
@@ -3639,36 +3625,36 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M22" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="N22" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="O22" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="P22" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="P22" s="6" t="s">
+      <c r="Q22" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="8"/>
       <c r="T22" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="U22" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="U22" s="8" t="s">
+      <c r="V22" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="W22" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="W22" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="X22" s="6" t="s">
         <v>53</v>
@@ -3683,16 +3669,16 @@
         <v>52</v>
       </c>
       <c r="AB22" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC22" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="AC22" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="AD22" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE22" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF22" s="6" t="s">
         <v>58</v>
@@ -3704,10 +3690,10 @@
         <v>60</v>
       </c>
       <c r="AI22" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="AJ22" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="AK22" s="6"/>
     </row>
@@ -3740,36 +3726,36 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M23" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="N23" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="O23" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="O23" s="8" t="s">
+      <c r="P23" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="P23" s="6" t="s">
-        <v>226</v>
-      </c>
       <c r="Q23" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R23" s="6"/>
       <c r="S23" s="8"/>
       <c r="T23" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="U23" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="V23" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="V23" s="6" t="s">
+      <c r="W23" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="W23" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="X23" s="6" t="s">
         <v>53</v>
@@ -3784,16 +3770,16 @@
         <v>68</v>
       </c>
       <c r="AB23" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC23" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="AC23" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="AD23" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE23" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF23" s="6" t="s">
         <v>58</v>
@@ -3805,10 +3791,10 @@
         <v>70</v>
       </c>
       <c r="AI23" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="AJ23" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="AK23" s="6"/>
     </row>
@@ -3839,54 +3825,54 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="M24" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="N24" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="O24" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="O24" s="8" t="s">
-        <v>240</v>
-      </c>
       <c r="P24" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q24" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="Q24" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="R24" s="6"/>
       <c r="S24" s="8"/>
       <c r="T24" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="U24" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="U24" s="8" t="s">
+      <c r="V24" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="V24" s="6" t="s">
-        <v>243</v>
-      </c>
       <c r="W24" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X24" s="6" t="s">
         <v>53</v>
       </c>
       <c r="Y24" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z24" s="6" t="s">
         <v>51</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC24" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="AC24" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="AD24" s="6" t="s">
         <v>57</v>
@@ -3905,7 +3891,7 @@
         <v>83</v>
       </c>
       <c r="AJ24" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AK24" s="6"/>
     </row>
@@ -3938,36 +3924,36 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="M25" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="M25" s="7" t="s">
+      <c r="N25" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="O25" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="O25" s="7" t="s">
+      <c r="P25" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="P25" s="6" t="s">
+      <c r="Q25" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="8"/>
       <c r="T25" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U25" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="V25" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="V25" s="6" t="s">
+      <c r="W25" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="W25" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="X25" s="6" t="s">
         <v>53</v>
@@ -3982,10 +3968,10 @@
         <v>52</v>
       </c>
       <c r="AB25" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC25" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="AC25" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="AD25" s="6" t="s">
         <v>57</v>
@@ -4003,10 +3989,10 @@
         <v>60</v>
       </c>
       <c r="AI25" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="AJ25" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="AK25" s="6"/>
     </row>
@@ -4039,36 +4025,36 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M26" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="O26" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="N26" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="O26" s="7" t="s">
+      <c r="P26" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q26" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>259</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="8"/>
       <c r="T26" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U26" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="V26" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="V26" s="6" t="s">
+      <c r="W26" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="W26" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="X26" s="6" t="s">
         <v>53</v>
@@ -4083,10 +4069,10 @@
         <v>68</v>
       </c>
       <c r="AB26" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC26" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="AC26" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="AD26" s="6" t="s">
         <v>57</v>
@@ -4104,10 +4090,10 @@
         <v>70</v>
       </c>
       <c r="AI26" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ26" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="AJ26" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="AK26" s="6"/>
     </row>
@@ -4138,60 +4124,60 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="M27" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="N27" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="N27" s="6" t="s">
+      <c r="O27" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="P27" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="P27" s="6" t="s">
+      <c r="Q27" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="Q27" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="8"/>
       <c r="T27" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="U27" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="U27" s="8" t="s">
+      <c r="V27" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="V27" s="6" t="s">
+      <c r="W27" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="W27" s="8" t="s">
-        <v>269</v>
       </c>
       <c r="X27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="Y27" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z27" s="6" t="s">
         <v>53</v>
       </c>
       <c r="AA27" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB27" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="AB27" s="6" t="s">
+      <c r="AC27" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="AC27" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="AD27" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE27" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF27" s="6" t="s">
         <v>58</v>
@@ -4201,10 +4187,10 @@
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AJ27" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="AJ27" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="AK27" s="6"/>
     </row>
@@ -4237,40 +4223,38 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="M28" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="M28" s="7" t="s">
+      <c r="N28" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="N28" s="6" t="s">
+      <c r="O28" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="O28" s="7" t="s">
+      <c r="P28" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="P28" s="6" t="s">
+      <c r="Q28" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="Q28" s="7" t="s">
+      <c r="R28" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="R28" s="6" t="s">
+      <c r="S28" s="8"/>
+      <c r="T28" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="S28" s="8" t="s">
+      <c r="U28" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="T28" s="6" t="s">
+      <c r="V28" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="U28" s="8" t="s">
+      <c r="W28" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="V28" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="W28" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="X28" s="6" t="s">
         <v>51</v>
@@ -4285,16 +4269,16 @@
         <v>54</v>
       </c>
       <c r="AB28" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC28" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="AC28" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="AD28" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE28" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF28" s="6" t="s">
         <v>58</v>
@@ -4306,10 +4290,10 @@
         <v>60</v>
       </c>
       <c r="AI28" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AJ28" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="AJ28" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="AK28" s="6"/>
     </row>
@@ -4342,40 +4326,38 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M29" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="N29" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>290</v>
-      </c>
       <c r="R29" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="S29" s="8"/>
+      <c r="T29" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="S29" s="8" t="s">
+      <c r="U29" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="T29" s="6" t="s">
+      <c r="V29" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="U29" s="8" t="s">
+      <c r="W29" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="V29" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="W29" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="X29" s="6" t="s">
         <v>51</v>
@@ -4390,16 +4372,16 @@
         <v>69</v>
       </c>
       <c r="AB29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC29" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="AC29" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="AD29" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF29" s="6" t="s">
         <v>58</v>
@@ -4411,10 +4393,10 @@
         <v>70</v>
       </c>
       <c r="AI29" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AJ29" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="AJ29" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="AK29" s="6"/>
     </row>
@@ -4445,36 +4427,36 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="N30" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="O30" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="P30" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="O30" s="7" t="s">
+      <c r="Q30" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="P30" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="Q30" s="8" t="s">
-        <v>296</v>
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="8"/>
       <c r="T30" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="U30" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="V30" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="U30" s="8" t="s">
+      <c r="W30" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="W30" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="X30" s="6" t="s">
         <v>51</v>
@@ -4489,16 +4471,16 @@
         <v>54</v>
       </c>
       <c r="AB30" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AC30" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AD30" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF30" s="6" t="s">
         <v>58</v>
@@ -4510,10 +4492,10 @@
         <v>60</v>
       </c>
       <c r="AI30" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AJ30" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AK30" s="6"/>
     </row>
@@ -4544,55 +4526,53 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="N31" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="O31" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="N31" s="6" t="s">
+      <c r="P31" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="O31" s="7" t="s">
+      <c r="Q31" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="R31" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="Q31" s="8" t="s">
+      <c r="S31" s="8"/>
+      <c r="T31" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="R31" s="6" t="s">
+      <c r="U31" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="S31" s="8" t="s">
+      <c r="V31" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="T31" s="6" t="s">
+      <c r="W31" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="U31" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="V31" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="W31" s="7" t="s">
-        <v>315</v>
       </c>
       <c r="X31" s="6" t="s">
         <v>53</v>
       </c>
       <c r="Y31" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z31" s="6" t="s">
         <v>51</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AB31" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="AC31" s="8" t="s">
         <v>56</v>
@@ -4611,7 +4591,7 @@
       </c>
       <c r="AH31" s="6"/>
       <c r="AI31" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="AJ31" s="6" t="s">
         <v>62</v>
@@ -4647,56 +4627,56 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="O32" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="P32" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="N32" s="6" t="s">
+      <c r="Q32" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="O32" s="7" t="s">
+      <c r="R32" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="S32" s="8"/>
       <c r="T32" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="U32" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="V32" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="W32" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="U32" s="8" t="s">
+      <c r="X32" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="V32" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="W32" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="Y32" s="7" t="s">
         <v>80</v>
       </c>
       <c r="Z32" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA32" s="7" t="s">
         <v>79</v>
       </c>
       <c r="AB32" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AC32" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="AD32" s="6" t="s">
         <v>57</v>
@@ -4714,10 +4694,10 @@
         <v>60</v>
       </c>
       <c r="AI32" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AJ32" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AK32" s="6"/>
     </row>
@@ -4750,56 +4730,56 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S33" s="8"/>
       <c r="T33" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="U33" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="V33" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="W33" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="U33" s="8" t="s">
+      <c r="X33" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="V33" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="W33" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="X33" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="Y33" s="7" t="s">
         <v>89</v>
       </c>
       <c r="Z33" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA33" s="7" t="s">
         <v>88</v>
       </c>
       <c r="AB33" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AC33" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="AD33" s="6" t="s">
         <v>57</v>
@@ -4817,10 +4797,10 @@
         <v>70</v>
       </c>
       <c r="AI33" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AJ33" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AK33" s="6"/>
     </row>
@@ -4853,40 +4833,40 @@
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="O34" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="P34" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="N34" s="6" t="s">
+      <c r="Q34" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="O34" s="7" t="s">
+      <c r="R34" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="P34" s="6" t="s">
+      <c r="S34" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="Q34" s="7" t="s">
+      <c r="T34" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="U34" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="S34" s="8" t="s">
+      <c r="V34" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="T34" s="6" t="s">
+      <c r="W34" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="U34" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="V34" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="W34" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="X34" s="6" t="s">
         <v>51</v>
@@ -4901,16 +4881,16 @@
         <v>54</v>
       </c>
       <c r="AB34" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AC34" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AD34" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE34" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF34" s="6" t="s">
         <v>58</v>
@@ -4922,10 +4902,10 @@
         <v>60</v>
       </c>
       <c r="AI34" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AJ34" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AK34" s="6"/>
     </row>
@@ -4958,40 +4938,40 @@
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="P35" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="S35" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="Q35" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="R35" s="6" t="s">
+      <c r="T35" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="U35" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="V35" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="T35" s="6" t="s">
+      <c r="W35" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="U35" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="V35" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="W35" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="X35" s="6" t="s">
         <v>51</v>
@@ -5006,16 +4986,16 @@
         <v>69</v>
       </c>
       <c r="AB35" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AC35" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AD35" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE35" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF35" s="6" t="s">
         <v>58</v>
@@ -5027,10 +5007,10 @@
         <v>70</v>
       </c>
       <c r="AI35" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AJ35" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AK35" s="6"/>
     </row>
@@ -5061,60 +5041,60 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="O36" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="M36" s="8" t="s">
+      <c r="P36" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="Q36" s="8" t="s">
         <v>355</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="P36" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q36" s="8" t="s">
-        <v>358</v>
       </c>
       <c r="R36" s="6"/>
       <c r="S36" s="8"/>
       <c r="T36" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="U36" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="V36" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="W36" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="U36" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="V36" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="W36" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="X36" s="6" t="s">
         <v>53</v>
       </c>
       <c r="Y36" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z36" s="6" t="s">
         <v>51</v>
       </c>
       <c r="AA36" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB36" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC36" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="AC36" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="AD36" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE36" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF36" s="6" t="s">
         <v>58</v>
@@ -5124,10 +5104,10 @@
       </c>
       <c r="AH36" s="6"/>
       <c r="AI36" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ36" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="AJ36" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="AK36" s="6"/>
     </row>
@@ -5160,36 +5140,36 @@
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="O37" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="P37" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="N37" s="6" t="s">
+      <c r="Q37" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="P37" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q37" s="7" t="s">
-        <v>368</v>
       </c>
       <c r="R37" s="6"/>
       <c r="S37" s="8"/>
       <c r="T37" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="U37" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="V37" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="W37" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="U37" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="V37" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="W37" s="8" t="s">
-        <v>372</v>
       </c>
       <c r="X37" s="6" t="s">
         <v>51</v>
@@ -5204,16 +5184,16 @@
         <v>54</v>
       </c>
       <c r="AB37" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AC37" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="AD37" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE37" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF37" s="6" t="s">
         <v>58</v>
@@ -5225,10 +5205,10 @@
         <v>60</v>
       </c>
       <c r="AI37" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="AJ37" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AK37" s="6"/>
     </row>
@@ -5261,36 +5241,36 @@
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="M38" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q38" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="N38" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="O38" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="P38" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q38" s="7" t="s">
-        <v>379</v>
       </c>
       <c r="R38" s="6"/>
       <c r="S38" s="8"/>
       <c r="T38" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="U38" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="W38" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="U38" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="V38" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="W38" s="8" t="s">
-        <v>372</v>
       </c>
       <c r="X38" s="6" t="s">
         <v>51</v>
@@ -5305,16 +5285,16 @@
         <v>69</v>
       </c>
       <c r="AB38" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AC38" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="AD38" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE38" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF38" s="6" t="s">
         <v>58</v>
@@ -5326,10 +5306,10 @@
         <v>70</v>
       </c>
       <c r="AI38" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="AJ38" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AK38" s="6"/>
     </row>
@@ -5362,62 +5342,62 @@
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="O39" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="M39" s="7" t="s">
+      <c r="P39" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q39" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="N39" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="O39" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="P39" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q39" s="7" t="s">
-        <v>384</v>
-      </c>
       <c r="R39" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S39" s="8"/>
       <c r="T39" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="U39" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="W39" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="U39" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="V39" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="W39" s="8" t="s">
-        <v>388</v>
-      </c>
       <c r="X39" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Y39" s="7" t="s">
         <v>54</v>
       </c>
       <c r="Z39" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA39" s="7" t="s">
         <v>52</v>
       </c>
       <c r="AB39" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AC39" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD39" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE39" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF39" s="6" t="s">
         <v>58</v>
@@ -5429,7 +5409,7 @@
         <v>60</v>
       </c>
       <c r="AI39" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AJ39" s="6" t="s">
         <v>84</v>
@@ -5465,62 +5445,62 @@
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="R40" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S40" s="8"/>
       <c r="T40" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="U40" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="W40" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="U40" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="V40" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="W40" s="8" t="s">
-        <v>388</v>
-      </c>
       <c r="X40" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Y40" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Z40" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA40" s="7" t="s">
         <v>68</v>
       </c>
       <c r="AB40" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AC40" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD40" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE40" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF40" s="6" t="s">
         <v>58</v>
@@ -5532,7 +5512,7 @@
         <v>70</v>
       </c>
       <c r="AI40" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AJ40" s="6" t="s">
         <v>84</v>
@@ -5568,40 +5548,38 @@
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="O41" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="M41" s="7" t="s">
+      <c r="P41" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="R41" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="N41" s="6" t="s">
+      <c r="S41" s="8"/>
+      <c r="T41" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="O41" s="7" t="s">
+      <c r="U41" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="P41" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="R41" s="6" t="s">
+      <c r="V41" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="S41" s="8" t="s">
+      <c r="W41" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="T41" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="U41" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="V41" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="W41" s="7" t="s">
-        <v>404</v>
       </c>
       <c r="X41" s="6" t="s">
         <v>53</v>
@@ -5616,16 +5594,16 @@
         <v>79</v>
       </c>
       <c r="AB41" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AC41" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD41" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE41" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF41" s="6" t="s">
         <v>58</v>
@@ -5637,7 +5615,7 @@
         <v>60</v>
       </c>
       <c r="AI41" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AJ41" s="6" t="s">
         <v>84</v>
@@ -5673,40 +5651,38 @@
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="N42" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="S42" s="8"/>
+      <c r="T42" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="O42" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q42" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="R42" s="6" t="s">
+      <c r="U42" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="V42" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="S42" s="8" t="s">
+      <c r="W42" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="T42" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="U42" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="V42" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="W42" s="7" t="s">
-        <v>404</v>
       </c>
       <c r="X42" s="6" t="s">
         <v>53</v>
@@ -5721,16 +5697,16 @@
         <v>88</v>
       </c>
       <c r="AB42" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AC42" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD42" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE42" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF42" s="6" t="s">
         <v>58</v>
@@ -5742,7 +5718,7 @@
         <v>70</v>
       </c>
       <c r="AI42" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AJ42" s="6" t="s">
         <v>84</v>

</xml_diff>